<commit_message>
Upgraded to asp.net mvc 5.0
</commit_message>
<xml_diff>
--- a/documentation/Business/Operating Costs/2017-10 October-Operating-Costs/Figlut Operating Costs 2017-10 October.xlsx
+++ b/documentation/Business/Operating Costs/2017-10 October-Operating-Costs/Figlut Operating Costs 2017-10 October.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9D816B-F788-47CD-A299-F219F876E13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="241" yWindow="106" windowWidth="14807" windowHeight="8007"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Item</t>
   </si>
@@ -43,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,6 +189,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -212,6 +241,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -387,78 +433,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B1">
+        <v>2017</v>
+      </c>
+      <c r="C1">
+        <v>2017</v>
+      </c>
+      <c r="D1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>320</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="C3">
+        <v>320</v>
+      </c>
+      <c r="D3">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>950</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="C4">
+        <v>950</v>
+      </c>
+      <c r="D4">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>174.15</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="C5">
+        <v>174.15</v>
+      </c>
+      <c r="D5">
+        <v>174.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>181.26</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>966.72</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
-        <f>SUM(B2:B7)</f>
+      <c r="B9" s="1">
+        <f>SUM(B3:B8)</f>
         <v>2592.13</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(C3:C8)</f>
+        <v>1444.15</v>
+      </c>
+      <c r="D9" s="1">
+        <f>SUM(D3:D8)</f>
+        <v>1788.15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>